<commit_message>
Final Versions of files to use
</commit_message>
<xml_diff>
--- a/forces.xlsx
+++ b/forces.xlsx
@@ -3,41 +3,34 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B060A4-C843-4A4E-AB79-F8521B96D9D3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298EF3C3-B3AE-4FC8-A9F4-7BB9060DA885}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>f1x</t>
+    <t>forces</t>
   </si>
   <si>
-    <t>f1y</t>
-  </si>
-  <si>
-    <t>f2x</t>
-  </si>
-  <si>
-    <t>f2y</t>
-  </si>
-  <si>
-    <t>f3x</t>
-  </si>
-  <si>
-    <t>f3y</t>
+    <t>canmove?</t>
   </si>
 </sst>
 </file>
@@ -61,9 +54,38 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -73,8 +95,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -355,63 +380,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="1" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <f>100000*COS(2*PI()*60/360)</f>
+        <v>50000.000000000015</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <f>-100000*SIN(2*PI()*60/360)</f>
+        <v>-86602.540378443853</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9" s="3">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>